<commit_message>
Sec 4.2 mostly done. On to the remaining sections
</commit_message>
<xml_diff>
--- a/figures/speedup/robustness_and_resource_requirements_fixed.xlsx
+++ b/figures/speedup/robustness_and_resource_requirements_fixed.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/philipc/Documents/Papers/In Progress/Newton-Krylov paper/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/philipc/Documents/Papers/In Progress/Newton-Krylov paper/paper-newton-krylov/figures/speedup/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{EFAE9522-771A-9541-96F3-9ADC5049F5AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38FD2494-2452-F44E-93D5-F3E6D3817289}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4520" yWindow="1600" windowWidth="45000" windowHeight="25780" xr2:uid="{21A20521-C10A-F24A-A87B-14ACABB684B6}"/>
   </bookViews>
@@ -982,11 +982,20 @@
                 <c:pt idx="36">
                   <c:v>85.710410094637226</c:v>
                 </c:pt>
+                <c:pt idx="38">
+                  <c:v>5.9999999999999938</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>28.874999999999993</c:v>
+                </c:pt>
                 <c:pt idx="51">
-                  <c:v>1.0994123408423115</c:v>
+                  <c:v>1.3994778067885119</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>1.7029354895412199</c:v>
+                  <c:v>1.6328490366028559</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1.2801209929849813</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2104,7 +2113,7 @@
   <dimension ref="A1:I60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G53" sqref="G53:I54"/>
+      <selection activeCell="G2" sqref="G2:I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2162,11 +2171,11 @@
         <v>79</v>
       </c>
       <c r="G2" s="3">
-        <f>3*B2</f>
+        <f t="shared" ref="G2:G22" si="0">3*B2</f>
         <v>1152</v>
       </c>
       <c r="I2">
-        <f>F2/D2</f>
+        <f t="shared" ref="I2:I18" si="1">F2/D2</f>
         <v>1.0128205128205128</v>
       </c>
     </row>
@@ -2187,11 +2196,11 @@
         <v>94</v>
       </c>
       <c r="G3" s="3">
-        <f>3*B3</f>
+        <f t="shared" si="0"/>
         <v>13122</v>
       </c>
       <c r="I3">
-        <f>F3/D3</f>
+        <f t="shared" si="1"/>
         <v>1.0930232558139534</v>
       </c>
     </row>
@@ -2212,7 +2221,7 @@
         <v>181</v>
       </c>
       <c r="G4" s="3">
-        <f>3*B4</f>
+        <f t="shared" si="0"/>
         <v>123462</v>
       </c>
       <c r="H4">
@@ -2220,7 +2229,7 @@
         <v>1.9999999999999978</v>
       </c>
       <c r="I4">
-        <f>F4/D4</f>
+        <f t="shared" si="1"/>
         <v>0.92820512820512824</v>
       </c>
     </row>
@@ -2241,7 +2250,7 @@
         <v>1289</v>
       </c>
       <c r="G5" s="3">
-        <f>3*B5</f>
+        <f t="shared" si="0"/>
         <v>1067742</v>
       </c>
       <c r="H5">
@@ -2249,7 +2258,7 @@
         <v>2.2499999999999996</v>
       </c>
       <c r="I5">
-        <f>F5/D5</f>
+        <f t="shared" si="1"/>
         <v>1.2126058325493885</v>
       </c>
     </row>
@@ -2270,7 +2279,7 @@
         <v>6174</v>
       </c>
       <c r="G6" s="3">
-        <f>3*B6</f>
+        <f t="shared" si="0"/>
         <v>8874702</v>
       </c>
       <c r="H6">
@@ -2278,7 +2287,7 @@
         <v>2.2439024390243905</v>
       </c>
       <c r="I6">
-        <f>F6/D6</f>
+        <f t="shared" si="1"/>
         <v>0.9182034503271862</v>
       </c>
     </row>
@@ -2299,7 +2308,7 @@
         <v>30601</v>
       </c>
       <c r="G7" s="3">
-        <f>3*B7</f>
+        <f t="shared" si="0"/>
         <v>72354222</v>
       </c>
       <c r="H7">
@@ -2307,7 +2316,7 @@
         <v>3.5637860082304527</v>
       </c>
       <c r="I7">
-        <f>F7/D7</f>
+        <f t="shared" si="1"/>
         <v>0.99983663333986805</v>
       </c>
     </row>
@@ -2331,11 +2340,11 @@
         <v>76</v>
       </c>
       <c r="G8" s="3">
-        <f>3*B8</f>
+        <f t="shared" si="0"/>
         <v>135</v>
       </c>
       <c r="I8">
-        <f>F8/D8</f>
+        <f t="shared" si="1"/>
         <v>1.0555555555555556</v>
       </c>
     </row>
@@ -2356,11 +2365,11 @@
         <v>81</v>
       </c>
       <c r="G9" s="3">
-        <f>3*B9</f>
+        <f t="shared" si="0"/>
         <v>1416</v>
       </c>
       <c r="I9">
-        <f>F9/D9</f>
+        <f t="shared" si="1"/>
         <v>1.0384615384615385</v>
       </c>
     </row>
@@ -2381,7 +2390,7 @@
         <v>124</v>
       </c>
       <c r="G10" s="3">
-        <f>3*B10</f>
+        <f t="shared" si="0"/>
         <v>12420</v>
       </c>
       <c r="H10">
@@ -2389,7 +2398,7 @@
         <v>7.9999999999999911</v>
       </c>
       <c r="I10">
-        <f>F10/D10</f>
+        <f t="shared" si="1"/>
         <v>0.81045751633986929</v>
       </c>
     </row>
@@ -2410,7 +2419,7 @@
         <v>660</v>
       </c>
       <c r="G11" s="3">
-        <f>3*B11</f>
+        <f t="shared" si="0"/>
         <v>104904</v>
       </c>
       <c r="H11">
@@ -2418,7 +2427,7 @@
         <v>21.285714285714285</v>
       </c>
       <c r="I11">
-        <f>F11/D11</f>
+        <f t="shared" si="1"/>
         <v>0.87533156498673736</v>
       </c>
     </row>
@@ -2439,7 +2448,7 @@
         <v>3661</v>
       </c>
       <c r="G12" s="3">
-        <f>3*B12</f>
+        <f t="shared" si="0"/>
         <v>861840</v>
       </c>
       <c r="H12">
@@ -2447,7 +2456,7 @@
         <v>28.357894736842105</v>
       </c>
       <c r="I12">
-        <f>F12/D12</f>
+        <f t="shared" si="1"/>
         <v>0.92848085214303833</v>
       </c>
     </row>
@@ -2468,7 +2477,7 @@
         <v>20348</v>
       </c>
       <c r="G13" s="3">
-        <f>3*B13</f>
+        <f t="shared" si="0"/>
         <v>7314726</v>
       </c>
       <c r="H13">
@@ -2476,7 +2485,7 @@
         <v>46.246963562753038</v>
       </c>
       <c r="I13">
-        <f>F13/D13</f>
+        <f t="shared" si="1"/>
         <v>0.9298117346006215</v>
       </c>
     </row>
@@ -2500,11 +2509,11 @@
         <v>85</v>
       </c>
       <c r="G14" s="3">
-        <f>3*B14</f>
+        <f t="shared" si="0"/>
         <v>1872</v>
       </c>
       <c r="I14">
-        <f>F14/D14</f>
+        <f t="shared" si="1"/>
         <v>1.0119047619047619</v>
       </c>
     </row>
@@ -2525,7 +2534,7 @@
         <v>141</v>
       </c>
       <c r="G15" s="3">
-        <f>3*B15</f>
+        <f t="shared" si="0"/>
         <v>14976</v>
       </c>
       <c r="H15">
@@ -2533,7 +2542,7 @@
         <v>6.999999999999992</v>
       </c>
       <c r="I15">
-        <f>F15/D15</f>
+        <f t="shared" si="1"/>
         <v>1.110236220472441</v>
       </c>
     </row>
@@ -2554,7 +2563,7 @@
         <v>723</v>
       </c>
       <c r="G16" s="3">
-        <f>3*B16</f>
+        <f t="shared" si="0"/>
         <v>119808</v>
       </c>
       <c r="H16">
@@ -2562,7 +2571,7 @@
         <v>13.299999999999997</v>
       </c>
       <c r="I16">
-        <f>F16/D16</f>
+        <f t="shared" si="1"/>
         <v>1.2980251346499103</v>
       </c>
     </row>
@@ -2583,7 +2592,7 @@
         <v>3547</v>
       </c>
       <c r="G17" s="3">
-        <f>3*B17</f>
+        <f t="shared" si="0"/>
         <v>958464</v>
       </c>
       <c r="H17">
@@ -2591,7 +2600,7 @@
         <v>18.935064935064936</v>
       </c>
       <c r="I17">
-        <f>F17/D17</f>
+        <f t="shared" si="1"/>
         <v>0.88146123260437381</v>
       </c>
     </row>
@@ -2612,7 +2621,7 @@
         <v>21827</v>
       </c>
       <c r="G18" s="3">
-        <f>3*B18</f>
+        <f t="shared" si="0"/>
         <v>7667712</v>
       </c>
       <c r="H18">
@@ -2620,7 +2629,7 @@
         <v>27.038263849229011</v>
       </c>
       <c r="I18">
-        <f>F18/D18</f>
+        <f t="shared" si="1"/>
         <v>0.95673709125975281</v>
       </c>
     </row>
@@ -2640,7 +2649,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="3">
-        <f>3*B19</f>
+        <f t="shared" si="0"/>
         <v>4860</v>
       </c>
     </row>
@@ -2657,7 +2666,7 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="3">
-        <f>3*B20</f>
+        <f t="shared" si="0"/>
         <v>38880</v>
       </c>
     </row>
@@ -2674,7 +2683,7 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="3">
-        <f>3*B21</f>
+        <f t="shared" si="0"/>
         <v>311040</v>
       </c>
     </row>
@@ -2691,7 +2700,7 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="3">
-        <f>3*B22</f>
+        <f t="shared" si="0"/>
         <v>2488320</v>
       </c>
     </row>
@@ -2715,11 +2724,11 @@
         <v>76</v>
       </c>
       <c r="G23" s="3">
-        <f>2*B23</f>
+        <f t="shared" ref="G23:G46" si="2">2*B23</f>
         <v>18</v>
       </c>
       <c r="I23">
-        <f>F23/D23</f>
+        <f t="shared" ref="I23:I40" si="3">F23/D23</f>
         <v>0.98701298701298701</v>
       </c>
     </row>
@@ -2740,11 +2749,11 @@
         <v>76</v>
       </c>
       <c r="G24" s="3">
-        <f>2*B24</f>
+        <f t="shared" si="2"/>
         <v>72</v>
       </c>
       <c r="I24">
-        <f>F24/D24</f>
+        <f t="shared" si="3"/>
         <v>0.98701298701298701</v>
       </c>
     </row>
@@ -2765,11 +2774,11 @@
         <v>78</v>
       </c>
       <c r="G25" s="3">
-        <f>2*B25</f>
+        <f t="shared" si="2"/>
         <v>288</v>
       </c>
       <c r="I25">
-        <f>F25/D25</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -2790,11 +2799,11 @@
         <v>84</v>
       </c>
       <c r="G26" s="3">
-        <f>2*B26</f>
+        <f t="shared" si="2"/>
         <v>1152</v>
       </c>
       <c r="I26">
-        <f>F26/D26</f>
+        <f t="shared" si="3"/>
         <v>1.024390243902439</v>
       </c>
     </row>
@@ -2815,11 +2824,11 @@
         <v>102</v>
       </c>
       <c r="G27" s="3">
-        <f>2*B27</f>
+        <f t="shared" si="2"/>
         <v>4608</v>
       </c>
       <c r="I27">
-        <f>F27/D27</f>
+        <f t="shared" si="3"/>
         <v>1.0851063829787233</v>
       </c>
     </row>
@@ -2840,7 +2849,7 @@
         <v>186</v>
       </c>
       <c r="G28" s="3">
-        <f>2*B28</f>
+        <f t="shared" si="2"/>
         <v>18432</v>
       </c>
       <c r="H28">
@@ -2848,7 +2857,7 @@
         <v>32.999999999999964</v>
       </c>
       <c r="I28">
-        <f>F28/D28</f>
+        <f t="shared" si="3"/>
         <v>1.2236842105263157</v>
       </c>
     </row>
@@ -2869,7 +2878,7 @@
         <v>392</v>
       </c>
       <c r="G29" s="3">
-        <f>2*B29</f>
+        <f t="shared" si="2"/>
         <v>73728</v>
       </c>
       <c r="H29">
@@ -2877,7 +2886,7 @@
         <v>221.99999999999991</v>
       </c>
       <c r="I29">
-        <f>F29/D29</f>
+        <f t="shared" si="3"/>
         <v>0.78873239436619713</v>
       </c>
     </row>
@@ -2898,7 +2907,7 @@
         <v>1950</v>
       </c>
       <c r="G30" s="3">
-        <f>2*B30</f>
+        <f t="shared" si="2"/>
         <v>294912</v>
       </c>
       <c r="H30">
@@ -2906,7 +2915,7 @@
         <v>237.09999999999997</v>
       </c>
       <c r="I30">
-        <f>F30/D30</f>
+        <f t="shared" si="3"/>
         <v>1.3347022587268993</v>
       </c>
     </row>
@@ -2930,11 +2939,11 @@
         <v>78</v>
       </c>
       <c r="G31" s="3">
-        <f>2*B31</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="I31">
-        <f>F31/D31</f>
+        <f t="shared" si="3"/>
         <v>0.96296296296296291</v>
       </c>
     </row>
@@ -2955,11 +2964,11 @@
         <v>78</v>
       </c>
       <c r="G32" s="3">
-        <f>2*B32</f>
+        <f t="shared" si="2"/>
         <v>72</v>
       </c>
       <c r="I32">
-        <f>F32/D32</f>
+        <f t="shared" si="3"/>
         <v>0.96296296296296291</v>
       </c>
     </row>
@@ -2980,15 +2989,15 @@
         <v>80</v>
       </c>
       <c r="G33" s="3">
-        <f>2*B33</f>
+        <f t="shared" si="2"/>
         <v>288</v>
       </c>
       <c r="H33">
-        <f>E33/(C33+0.000000000000001)</f>
+        <f t="shared" ref="H33:H40" si="4">E33/(C33+0.000000000000001)</f>
         <v>1.6666666666666661</v>
       </c>
       <c r="I33">
-        <f>F33/D33</f>
+        <f t="shared" si="3"/>
         <v>0.95238095238095233</v>
       </c>
     </row>
@@ -3009,15 +3018,15 @@
         <v>91</v>
       </c>
       <c r="G34" s="3">
-        <f>2*B34</f>
+        <f t="shared" si="2"/>
         <v>1152</v>
       </c>
       <c r="H34">
-        <f>E34/(C34+0.000000000000001)</f>
+        <f t="shared" si="4"/>
         <v>2.8888888888888884</v>
       </c>
       <c r="I34">
-        <f>F34/D34</f>
+        <f t="shared" si="3"/>
         <v>0.93814432989690721</v>
       </c>
     </row>
@@ -3038,15 +3047,15 @@
         <v>132</v>
       </c>
       <c r="G35" s="3">
-        <f>2*B35</f>
+        <f t="shared" si="2"/>
         <v>4608</v>
       </c>
       <c r="H35">
-        <f>E35/(C35+0.000000000000001)</f>
+        <f t="shared" si="4"/>
         <v>4.882352941176471</v>
       </c>
       <c r="I35">
-        <f>F35/D35</f>
+        <f t="shared" si="3"/>
         <v>0.91666666666666663</v>
       </c>
     </row>
@@ -3067,15 +3076,15 @@
         <v>357</v>
       </c>
       <c r="G36" s="3">
-        <f>2*B36</f>
+        <f t="shared" si="2"/>
         <v>18432</v>
       </c>
       <c r="H36">
-        <f>E36/(C36+0.000000000000001)</f>
+        <f t="shared" si="4"/>
         <v>8.5341614906832302</v>
       </c>
       <c r="I36">
-        <f>F36/D36</f>
+        <f t="shared" si="3"/>
         <v>1.39453125</v>
       </c>
     </row>
@@ -3096,15 +3105,15 @@
         <v>1053</v>
       </c>
       <c r="G37" s="3">
-        <f>2*B37</f>
+        <f t="shared" si="2"/>
         <v>73728</v>
       </c>
       <c r="H37">
-        <f>E37/(C37+0.000000000000001)</f>
+        <f t="shared" si="4"/>
         <v>18.594186046511627</v>
       </c>
       <c r="I37">
-        <f>F37/D37</f>
+        <f t="shared" si="3"/>
         <v>1.9007220216606497</v>
       </c>
     </row>
@@ -3125,15 +3134,15 @@
         <v>2341</v>
       </c>
       <c r="G38" s="3">
-        <f>2*B38</f>
+        <f t="shared" si="2"/>
         <v>294912</v>
       </c>
       <c r="H38">
-        <f>E38/(C38+0.000000000000001)</f>
+        <f t="shared" si="4"/>
         <v>85.710410094637226</v>
       </c>
       <c r="I38">
-        <f>F38/D38</f>
+        <f t="shared" si="3"/>
         <v>0.82226905514576742</v>
       </c>
     </row>
@@ -3144,8 +3153,12 @@
       <c r="B39" s="2">
         <v>9</v>
       </c>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
+      <c r="C39" s="2">
+        <v>0</v>
+      </c>
+      <c r="D39" s="2">
+        <v>78</v>
+      </c>
       <c r="E39" s="2">
         <v>3</v>
       </c>
@@ -3153,7 +3166,7 @@
         <v>78</v>
       </c>
       <c r="G39" s="3">
-        <f>2*B39</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
     </row>
@@ -3161,8 +3174,12 @@
       <c r="B40" s="2">
         <v>36</v>
       </c>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
+      <c r="C40" s="2">
+        <v>1</v>
+      </c>
+      <c r="D40" s="2">
+        <v>79</v>
+      </c>
       <c r="E40" s="2">
         <v>6</v>
       </c>
@@ -3170,8 +3187,16 @@
         <v>79</v>
       </c>
       <c r="G40" s="3">
-        <f>2*B40</f>
+        <f t="shared" si="2"/>
         <v>72</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="4"/>
+        <v>5.9999999999999938</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
@@ -3187,7 +3212,7 @@
         <v>82</v>
       </c>
       <c r="G41" s="3">
-        <f>2*B41</f>
+        <f t="shared" si="2"/>
         <v>288</v>
       </c>
     </row>
@@ -3195,8 +3220,12 @@
       <c r="B42" s="2">
         <v>576</v>
       </c>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
+      <c r="C42" s="2">
+        <v>8</v>
+      </c>
+      <c r="D42" s="2">
+        <v>90</v>
+      </c>
       <c r="E42" s="2">
         <v>231</v>
       </c>
@@ -3204,8 +3233,16 @@
         <v>104</v>
       </c>
       <c r="G42" s="3">
-        <f>2*B42</f>
+        <f t="shared" si="2"/>
         <v>1152</v>
+      </c>
+      <c r="H42">
+        <f t="shared" ref="H41:H42" si="5">E42/(C42+0.000000000000001)</f>
+        <v>28.874999999999993</v>
+      </c>
+      <c r="I42">
+        <f t="shared" ref="I41:I42" si="6">F42/D42</f>
+        <v>1.1555555555555554</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
@@ -3221,7 +3258,7 @@
         <v>180</v>
       </c>
       <c r="G43" s="3">
-        <f>2*B43</f>
+        <f t="shared" si="2"/>
         <v>4608</v>
       </c>
     </row>
@@ -3238,7 +3275,7 @@
         <v>451</v>
       </c>
       <c r="G44" s="3">
-        <f>2*B44</f>
+        <f t="shared" si="2"/>
         <v>18432</v>
       </c>
     </row>
@@ -3255,7 +3292,7 @@
         <v>1396</v>
       </c>
       <c r="G45" s="3">
-        <f>2*B45</f>
+        <f t="shared" si="2"/>
         <v>73728</v>
       </c>
     </row>
@@ -3272,7 +3309,7 @@
         <v>3466</v>
       </c>
       <c r="G46" s="3">
-        <f>2*B46</f>
+        <f t="shared" si="2"/>
         <v>294912</v>
       </c>
     </row>
@@ -3292,7 +3329,7 @@
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
       <c r="G47" s="3">
-        <f>3*B47</f>
+        <f t="shared" ref="G47:G52" si="7">3*B47</f>
         <v>810</v>
       </c>
     </row>
@@ -3309,7 +3346,7 @@
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
       <c r="G48" s="3">
-        <f>3*B48</f>
+        <f t="shared" si="7"/>
         <v>6480</v>
       </c>
     </row>
@@ -3326,7 +3363,7 @@
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
       <c r="G49" s="3">
-        <f>3*B49</f>
+        <f t="shared" si="7"/>
         <v>51840</v>
       </c>
     </row>
@@ -3343,7 +3380,7 @@
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
       <c r="G50" s="3">
-        <f>3*B50</f>
+        <f t="shared" si="7"/>
         <v>414720</v>
       </c>
     </row>
@@ -3357,7 +3394,7 @@
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
       <c r="G51" s="3">
-        <f>3*B51</f>
+        <f t="shared" si="7"/>
         <v>966483</v>
       </c>
     </row>
@@ -3368,7 +3405,7 @@
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
       <c r="G52" s="3">
-        <f>3*B52</f>
+        <f t="shared" si="7"/>
         <v>7479897</v>
       </c>
     </row>
@@ -3381,28 +3418,28 @@
         <v>1408</v>
       </c>
       <c r="C53" s="2">
-        <v>4084</v>
+        <v>3830</v>
       </c>
       <c r="D53" s="2">
-        <v>758</v>
+        <v>748</v>
       </c>
       <c r="E53" s="2">
-        <v>4490</v>
+        <v>5360</v>
       </c>
       <c r="F53" s="2">
-        <v>732</v>
+        <v>738</v>
       </c>
       <c r="G53" s="3">
         <f>2*B53+1252</f>
         <v>4068</v>
       </c>
       <c r="H53">
-        <f t="shared" ref="H53:H54" si="0">E53/(C53+0.000000000000001)</f>
-        <v>1.0994123408423115</v>
+        <f t="shared" ref="H53:H55" si="8">E53/(C53+0.000000000000001)</f>
+        <v>1.3994778067885119</v>
       </c>
       <c r="I53">
         <f>F53/D53</f>
-        <v>0.96569920844327173</v>
+        <v>0.9866310160427807</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
@@ -3411,28 +3448,28 @@
         <v>5632</v>
       </c>
       <c r="C54" s="2">
-        <v>28445</v>
+        <v>32074</v>
       </c>
       <c r="D54" s="2">
-        <v>777</v>
+        <v>834</v>
       </c>
       <c r="E54" s="2">
-        <v>48440</v>
+        <v>52372</v>
       </c>
       <c r="F54" s="2">
-        <v>760</v>
+        <v>775</v>
       </c>
       <c r="G54" s="3">
         <f>2*B54+5008</f>
         <v>16272</v>
       </c>
       <c r="H54">
-        <f t="shared" si="0"/>
-        <v>1.7029354895412199</v>
+        <f t="shared" si="8"/>
+        <v>1.6328490366028559</v>
       </c>
       <c r="I54">
         <f>F54/D54</f>
-        <v>0.97812097812097809</v>
+        <v>0.92925659472422062</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
@@ -3441,17 +3478,29 @@
         <v>22528</v>
       </c>
       <c r="C55" s="2">
-        <v>154237</v>
+        <v>170919</v>
       </c>
       <c r="D55" s="2">
-        <v>729</v>
-      </c>
-      <c r="E55" s="2"/>
-      <c r="F55" s="2"/>
+        <v>785</v>
+      </c>
+      <c r="E55" s="2">
+        <v>218797</v>
+      </c>
+      <c r="F55" s="2">
+        <v>748</v>
+      </c>
       <c r="G55" s="3">
         <f>2*B55+20032</f>
         <v>65088</v>
       </c>
+      <c r="H55">
+        <f t="shared" si="8"/>
+        <v>1.2801209929849813</v>
+      </c>
+      <c r="I55">
+        <f>F55/D55</f>
+        <v>0.95286624203821657</v>
+      </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="G58" t="s">
@@ -3468,7 +3517,7 @@
       </c>
       <c r="H59">
         <f>MIN(H2:H55)</f>
-        <v>1.0994123408423115</v>
+        <v>1.2801209929849813</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
@@ -3477,7 +3526,7 @@
       </c>
       <c r="H60">
         <f>AVERAGE(H2:H55)</f>
-        <v>34.669591468513289</v>
+        <v>32.068680914684549</v>
       </c>
     </row>
   </sheetData>

</xml_diff>